<commit_message>
diagramas de casos de uso de baixo nivel
</commit_message>
<xml_diff>
--- a/FaceOculta/ES2N-Requisitos Funcionais v5.0.xlsx
+++ b/FaceOculta/ES2N-Requisitos Funcionais v5.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ES2N\FaceOculta\Revisao03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ES2N\FaceOculta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2FDBDB-5DFD-4EB3-93C0-A8060CF183A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCADAF0E-E2B8-4704-9AB5-5682944D831E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t xml:space="preserve">LISTA DE REQUISITOS FUNCIONAIS </t>
   </si>
@@ -146,9 +146,6 @@
     <t>RF05</t>
   </si>
   <si>
-    <t>Gerenciar Perfil</t>
-  </si>
-  <si>
     <t>RF06</t>
   </si>
   <si>
@@ -316,6 +313,41 @@
   </si>
   <si>
     <t>Sistema;Usuário Autenticado(Professor,Administrador,Aluno);Visitante</t>
+  </si>
+  <si>
+    <t>Vistante</t>
+  </si>
+  <si>
+    <t>RF15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> executar RF15</t>
+    </r>
+  </si>
+  <si>
+    <t>Enviar Aprovação Cadastro</t>
+  </si>
+  <si>
+    <t>Editar Perfil</t>
+  </si>
+  <si>
+    <t>O sistema envia um email que o cadastro foi aprovado ou recusado</t>
   </si>
 </sst>
 </file>
@@ -437,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,10 +497,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -689,7 +718,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -753,7 +782,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3"/>
       <c r="F8" s="3"/>
@@ -814,13 +843,13 @@
         <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="46.5" x14ac:dyDescent="0.35">
@@ -834,7 +863,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>18</v>
@@ -848,11 +877,11 @@
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>14</v>
@@ -870,7 +899,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>14</v>
@@ -882,13 +911,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>14</v>
@@ -897,16 +926,16 @@
     </row>
     <row r="16" spans="1:27" ht="116.25" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>18</v>
@@ -915,16 +944,16 @@
     </row>
     <row r="17" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>18</v>
@@ -933,16 +962,16 @@
     </row>
     <row r="18" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>18</v>
@@ -951,16 +980,16 @@
     </row>
     <row r="19" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>18</v>
@@ -969,72 +998,72 @@
     </row>
     <row r="20" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="C21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>18</v>
@@ -1051,28 +1080,40 @@
     </row>
     <row r="25" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="F25" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>